<commit_message>
Corrected salary tax on examples and rerun them
</commit_message>
<xml_diff>
--- a/tests/Feature/config/example_simple_tenpercent.xlsx
+++ b/tests/Feature/config/example_simple_tenpercent.xlsx
@@ -1212,7 +1212,7 @@
     <col min="4" max="4" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
@@ -3846,7 +3846,7 @@
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
-        <v>0.0</v>
+        <v>264000.0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1">
@@ -3888,7 +3888,7 @@
       </c>
       <c r="X38" s="2"/>
       <c r="Y38" s="1">
-        <v>4743.4</v>
+        <v>-259256.6</v>
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
@@ -3925,7 +3925,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="8">
-        <v>0.0</v>
+        <v>290400.0</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="8">
@@ -3967,7 +3967,7 @@
       </c>
       <c r="X39" s="9"/>
       <c r="Y39" s="8">
-        <v>22836.2</v>
+        <v>-267563.8</v>
       </c>
       <c r="Z39" s="9"/>
       <c r="AA39" s="8">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="11">
-        <v>0.0</v>
+        <v>319440.0</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="11">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="X40" s="12"/>
       <c r="Y40" s="11">
-        <v>42738.5</v>
+        <v>-276701.5</v>
       </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
-        <v>0.0</v>
+        <v>351384.0</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="X41" s="2"/>
       <c r="Y41" s="1">
-        <v>64630.7</v>
+        <v>-286753.3</v>
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
@@ -4162,7 +4162,7 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
-        <v>0.0</v>
+        <v>386522.4</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="1">
-        <v>88711.9</v>
+        <v>-297810.5</v>
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
-        <v>0.0</v>
+        <v>425174.75</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="1">
-        <v>115201.0</v>
+        <v>-309973.75</v>
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
@@ -4320,7 +4320,7 @@
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
-        <v>0.0</v>
+        <v>467692.5</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1">
@@ -4362,7 +4362,7 @@
       </c>
       <c r="X44" s="2"/>
       <c r="Y44" s="1">
-        <v>144341.1</v>
+        <v>-323351.4</v>
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
-        <v>0.0</v>
+        <v>514461.75</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="1">
-        <v>176394.0</v>
+        <v>-338067.75</v>
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
-        <v>0.0</v>
+        <v>565908.2</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="1">
-        <v>211652.3</v>
+        <v>-354255.9</v>
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
@@ -4557,7 +4557,7 @@
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
-        <v>0.0</v>
+        <v>622498.8</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="1">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="1">
-        <v>249750.3925</v>
+        <v>-372748.4075</v>
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
@@ -4636,7 +4636,7 @@
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
-        <v>0.0</v>
+        <v>684748.9</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="1">
-        <v>290644.3325</v>
+        <v>-394104.5675</v>
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
-        <v>0.0</v>
+        <v>753223.9</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="1">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="1">
-        <v>335628.325</v>
+        <v>-417595.575</v>
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
@@ -4794,7 +4794,7 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
-        <v>0.0</v>
+        <v>828546.4</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="1">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="X50" s="2"/>
       <c r="Y50" s="1">
-        <v>385109.2875</v>
+        <v>-443437.1125</v>
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
-        <v>0.0</v>
+        <v>911401.15</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="1">
@@ -4915,7 +4915,7 @@
       </c>
       <c r="X51" s="2"/>
       <c r="Y51" s="1">
-        <v>439538.565</v>
+        <v>-471862.585</v>
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
@@ -4952,7 +4952,7 @@
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
-        <v>0.0</v>
+        <v>1002541.1</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="1">
@@ -4994,7 +4994,7 @@
       </c>
       <c r="X52" s="2"/>
       <c r="Y52" s="1">
-        <v>499410.6625</v>
+        <v>-503130.4375</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="13">
-        <v>0.0</v>
+        <v>65285.5</v>
       </c>
       <c r="H53" s="14"/>
       <c r="I53" s="13">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="X53" s="14"/>
       <c r="Y53" s="13">
-        <v>-1509748.4625</v>
+        <v>-1575033.9625</v>
       </c>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
@@ -5110,7 +5110,7 @@
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
-        <v>0.0</v>
+        <v>71814.5</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="1">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="X54" s="2"/>
       <c r="Y54" s="1">
-        <v>-1644804.5</v>
+        <v>-1716619.0</v>
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
@@ -5189,7 +5189,7 @@
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
-        <v>0.0</v>
+        <v>78995.5</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="1">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="X55" s="2"/>
       <c r="Y55" s="1">
-        <v>-1793366.73</v>
+        <v>-1872362.23</v>
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
-        <v>0.0</v>
+        <v>86895.5</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="1">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="X56" s="2"/>
       <c r="Y56" s="1">
-        <v>-1956784.4825</v>
+        <v>-2043679.9825</v>
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
@@ -5347,7 +5347,7 @@
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="13">
-        <v>0.0</v>
+        <v>194585.0</v>
       </c>
       <c r="H57" s="14"/>
       <c r="I57" s="13">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="X57" s="14"/>
       <c r="Y57" s="13">
-        <v>-1938544.02</v>
+        <v>-2133129.02</v>
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>0.0</v>
+        <v>214043.5</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="1">
@@ -5468,7 +5468,7 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="1">
-        <v>-1941006.4625</v>
+        <v>-2155049.9625</v>
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
@@ -5505,7 +5505,7 @@
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>0.0</v>
+        <v>235447.5</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="1">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="1">
-        <v>-2138507.1475</v>
+        <v>-2373954.6475</v>
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
@@ -5584,7 +5584,7 @@
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>0.0</v>
+        <v>258992.5</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="1">
@@ -5626,7 +5626,7 @@
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="1">
-        <v>-2355758.355</v>
+        <v>-2614750.855</v>
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="1">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>0.0</v>
+        <v>284891.4</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1">
@@ -5705,7 +5705,7 @@
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="1">
-        <v>-2594734.4525</v>
+        <v>-2879625.8525</v>
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="1">
@@ -5742,7 +5742,7 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>0.0</v>
+        <v>313380.6</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="1">
-        <v>-2857607.23</v>
+        <v>-3170987.83</v>
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="1">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>0.0</v>
+        <v>344718.55</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="1">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="X63" s="2"/>
       <c r="Y63" s="1">
-        <v>-3146768.17</v>
+        <v>-3491486.72</v>
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="1">
@@ -5900,7 +5900,7 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>0.0</v>
+        <v>379190.45</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="1">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="X64" s="2"/>
       <c r="Y64" s="1">
-        <v>-3464845.12</v>
+        <v>-3844035.57</v>
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="1">
@@ -5979,7 +5979,7 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>0.0</v>
+        <v>417109.8</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="1">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" s="1">
-        <v>-3814729.6825</v>
+        <v>-4231839.4825</v>
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="1">
@@ -6058,7 +6058,7 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>0.0</v>
+        <v>458821.05</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="X66" s="2"/>
       <c r="Y66" s="1">
-        <v>-4199602.55</v>
+        <v>-4658423.6</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="1">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>0.0</v>
+        <v>504702.7</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="1">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" s="1">
-        <v>-4622964.595</v>
+        <v>-5127667.295</v>
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="1">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>0.0</v>
+        <v>324841.05</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="1">
@@ -6258,7 +6258,7 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="1">
-        <v>-5549325.665</v>
+        <v>-5874166.715</v>
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="1">
@@ -6295,7 +6295,7 @@
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>0.0</v>
+        <v>357325.35</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="1">
@@ -6337,7 +6337,7 @@
       </c>
       <c r="X69" s="2"/>
       <c r="Y69" s="1">
-        <v>-6107657.2875</v>
+        <v>-6464982.6375</v>
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="1">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>0.0</v>
+        <v>393057.95</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="1">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" s="1">
-        <v>-6721823.215</v>
+        <v>-7114881.165</v>
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="1">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>0.0</v>
+        <v>432363.5</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="1">
@@ -6495,7 +6495,7 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" s="1">
-        <v>-7397405.3675</v>
+        <v>-7829768.8675</v>
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="1">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="5">
-        <v>0.0</v>
+        <v>475599.25</v>
       </c>
       <c r="H72" s="16"/>
       <c r="I72" s="5">
@@ -6574,7 +6574,7 @@
       </c>
       <c r="X72" s="16"/>
       <c r="Y72" s="5">
-        <v>-8140547.545</v>
+        <v>-8616146.795</v>
       </c>
       <c r="Z72" s="16"/>
       <c r="AA72" s="5">
@@ -7677,7 +7677,7 @@
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -7882,7 +7882,9 @@
       <c r="G6" s="1">
         <v>0.0</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
@@ -7950,7 +7952,9 @@
       <c r="G7" s="1">
         <v>0.0</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
@@ -8018,7 +8022,9 @@
       <c r="G8" s="1">
         <v>0.0</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
@@ -8086,7 +8092,9 @@
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
@@ -8154,7 +8162,9 @@
       <c r="G10" s="1">
         <v>0.0</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
@@ -8222,7 +8232,9 @@
       <c r="G11" s="1">
         <v>0.0</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
@@ -8290,7 +8302,9 @@
       <c r="G12" s="1">
         <v>0.0</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
@@ -8358,7 +8372,9 @@
       <c r="G13" s="1">
         <v>0.0</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
@@ -8426,7 +8442,9 @@
       <c r="G14" s="1">
         <v>0.0</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
@@ -8494,7 +8512,9 @@
       <c r="G15" s="1">
         <v>0.0</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
@@ -8562,7 +8582,9 @@
       <c r="G16" s="1">
         <v>0.0</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
@@ -8630,7 +8652,9 @@
       <c r="G17" s="1">
         <v>0.0</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
@@ -8698,7 +8722,9 @@
       <c r="G18" s="1">
         <v>0.0</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
@@ -8766,7 +8792,9 @@
       <c r="G19" s="1">
         <v>0.0</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
@@ -8834,7 +8862,9 @@
       <c r="G20" s="1">
         <v>0.0</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
@@ -8902,7 +8932,9 @@
       <c r="G21" s="1">
         <v>0.0</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
@@ -8970,7 +9002,9 @@
       <c r="G22" s="1">
         <v>0.0</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
@@ -9038,7 +9072,9 @@
       <c r="G23" s="1">
         <v>0.0</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1"/>
@@ -9106,7 +9142,9 @@
       <c r="G24" s="1">
         <v>0.0</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
@@ -9174,7 +9212,9 @@
       <c r="G25" s="1">
         <v>0.0</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="2"/>
       <c r="K25" s="1"/>
@@ -9242,7 +9282,9 @@
       <c r="G26" s="1">
         <v>0.0</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="2"/>
       <c r="K26" s="1"/>
@@ -9310,7 +9352,9 @@
       <c r="G27" s="1">
         <v>0.0</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
@@ -9378,7 +9422,9 @@
       <c r="G28" s="1">
         <v>0.0</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
       <c r="K28" s="1"/>
@@ -9446,7 +9492,9 @@
       <c r="G29" s="1">
         <v>0.0</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1"/>
@@ -9514,7 +9562,9 @@
       <c r="G30" s="1">
         <v>0.0</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
       <c r="K30" s="1"/>
@@ -9582,7 +9632,9 @@
       <c r="G31" s="1">
         <v>0.0</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1"/>
@@ -9650,7 +9702,9 @@
       <c r="G32" s="1">
         <v>0.0</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="2"/>
       <c r="K32" s="1"/>
@@ -9718,7 +9772,9 @@
       <c r="G33" s="1">
         <v>0.0</v>
       </c>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1"/>
@@ -9786,7 +9842,9 @@
       <c r="G34" s="1">
         <v>0.0</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="2"/>
       <c r="K34" s="1"/>
@@ -9854,7 +9912,9 @@
       <c r="G35" s="1">
         <v>0.0</v>
       </c>
-      <c r="H35" s="2"/>
+      <c r="H35" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1"/>
@@ -9922,7 +9982,9 @@
       <c r="G36" s="1">
         <v>0.0</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="2"/>
       <c r="K36" s="1"/>
@@ -9990,7 +10052,9 @@
       <c r="G37" s="1">
         <v>0.0</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1"/>
@@ -10060,9 +10124,11 @@
         <v>0.1</v>
       </c>
       <c r="G38" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H38" s="2"/>
+        <v>264000.0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="2"/>
       <c r="K38" s="1"/>
@@ -10092,7 +10158,7 @@
       </c>
       <c r="X38" s="2"/>
       <c r="Y38" s="1">
-        <v>330000.0</v>
+        <v>66000.0</v>
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
@@ -10132,9 +10198,11 @@
         <v>0.1</v>
       </c>
       <c r="G39" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="9"/>
+        <v>290400.0</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I39" s="8"/>
       <c r="J39" s="9"/>
       <c r="K39" s="8"/>
@@ -10164,7 +10232,7 @@
       </c>
       <c r="X39" s="9"/>
       <c r="Y39" s="8">
-        <v>363000.0</v>
+        <v>72600.0</v>
       </c>
       <c r="Z39" s="9"/>
       <c r="AA39" s="8">
@@ -10205,9 +10273,11 @@
         <v>0.1</v>
       </c>
       <c r="G40" s="11">
-        <v>0.0</v>
-      </c>
-      <c r="H40" s="12"/>
+        <v>319440.0</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0.5</v>
+      </c>
       <c r="I40" s="11"/>
       <c r="J40" s="12"/>
       <c r="K40" s="11"/>
@@ -10237,7 +10307,7 @@
       </c>
       <c r="X40" s="12"/>
       <c r="Y40" s="11">
-        <v>399300.0</v>
+        <v>79860.0</v>
       </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
@@ -10278,9 +10348,11 @@
         <v>0.1</v>
       </c>
       <c r="G41" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H41" s="2"/>
+        <v>351384.0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="2"/>
       <c r="K41" s="1"/>
@@ -10310,7 +10382,7 @@
       </c>
       <c r="X41" s="2"/>
       <c r="Y41" s="1">
-        <v>439230.0</v>
+        <v>87846.0</v>
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
@@ -10350,9 +10422,11 @@
         <v>0.1</v>
       </c>
       <c r="G42" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>386522.4</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="2"/>
       <c r="K42" s="1"/>
@@ -10382,7 +10456,7 @@
       </c>
       <c r="X42" s="2"/>
       <c r="Y42" s="1">
-        <v>483153.0</v>
+        <v>96630.6</v>
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
@@ -10422,9 +10496,11 @@
         <v>0.1</v>
       </c>
       <c r="G43" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H43" s="2"/>
+        <v>425174.75</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="2"/>
       <c r="K43" s="1"/>
@@ -10454,7 +10530,7 @@
       </c>
       <c r="X43" s="2"/>
       <c r="Y43" s="1">
-        <v>531468.3</v>
+        <v>106293.55</v>
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
@@ -10494,9 +10570,11 @@
         <v>0.1</v>
       </c>
       <c r="G44" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H44" s="2"/>
+        <v>467692.5</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="2"/>
       <c r="K44" s="1"/>
@@ -10526,7 +10604,7 @@
       </c>
       <c r="X44" s="2"/>
       <c r="Y44" s="1">
-        <v>584615.9</v>
+        <v>116923.4</v>
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
@@ -10566,9 +10644,11 @@
         <v>0.1</v>
       </c>
       <c r="G45" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H45" s="2"/>
+        <v>514461.75</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="2"/>
       <c r="K45" s="1"/>
@@ -10598,7 +10678,7 @@
       </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="1">
-        <v>643077.6</v>
+        <v>128615.85</v>
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
@@ -10638,9 +10718,11 @@
         <v>0.1</v>
       </c>
       <c r="G46" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H46" s="2"/>
+        <v>565908.2</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="2"/>
       <c r="K46" s="1"/>
@@ -10670,7 +10752,7 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="1">
-        <v>707385.8</v>
+        <v>141477.6</v>
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
@@ -10710,9 +10792,11 @@
         <v>0.1</v>
       </c>
       <c r="G47" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H47" s="2"/>
+        <v>622498.8</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="2"/>
       <c r="K47" s="1"/>
@@ -10742,7 +10826,7 @@
       </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="1">
-        <v>778123.5</v>
+        <v>155624.7</v>
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
@@ -10782,9 +10866,11 @@
         <v>0.1</v>
       </c>
       <c r="G48" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H48" s="2"/>
+        <v>684748.9</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="2"/>
       <c r="K48" s="1"/>
@@ -10814,7 +10900,7 @@
       </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="1">
-        <v>855936.4</v>
+        <v>171187.5</v>
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
@@ -10854,9 +10940,11 @@
         <v>0.1</v>
       </c>
       <c r="G49" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H49" s="2"/>
+        <v>753223.9</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="2"/>
       <c r="K49" s="1"/>
@@ -10886,7 +10974,7 @@
       </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="1">
-        <v>941530.7</v>
+        <v>188306.8</v>
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
@@ -10926,9 +11014,11 @@
         <v>0.1</v>
       </c>
       <c r="G50" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H50" s="2"/>
+        <v>828546.4</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="2"/>
       <c r="K50" s="1"/>
@@ -10958,7 +11048,7 @@
       </c>
       <c r="X50" s="2"/>
       <c r="Y50" s="1">
-        <v>1035684.1</v>
+        <v>207137.7</v>
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
@@ -10998,9 +11088,11 @@
         <v>0.1</v>
       </c>
       <c r="G51" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H51" s="2"/>
+        <v>911401.15</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I51" s="1"/>
       <c r="J51" s="2"/>
       <c r="K51" s="1"/>
@@ -11030,7 +11122,7 @@
       </c>
       <c r="X51" s="2"/>
       <c r="Y51" s="1">
-        <v>1139252.4</v>
+        <v>227851.25</v>
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
@@ -11070,9 +11162,11 @@
         <v>0.1</v>
       </c>
       <c r="G52" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H52" s="2"/>
+        <v>1002541.1</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52" s="1"/>
@@ -11102,7 +11196,7 @@
       </c>
       <c r="X52" s="2"/>
       <c r="Y52" s="1">
-        <v>1253177.2</v>
+        <v>250636.1</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
@@ -11140,9 +11234,11 @@
         <v>0.1</v>
       </c>
       <c r="G53" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H53" s="14"/>
+        <v>65285.5</v>
+      </c>
+      <c r="H53" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I53" s="13"/>
       <c r="J53" s="14"/>
       <c r="K53" s="13"/>
@@ -11172,7 +11268,7 @@
       </c>
       <c r="X53" s="14"/>
       <c r="Y53" s="13">
-        <v>-696524.5</v>
+        <v>-761810.0</v>
       </c>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
@@ -11211,9 +11307,11 @@
         <v>0.1</v>
       </c>
       <c r="G54" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H54" s="2"/>
+        <v>71814.5</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I54" s="1"/>
       <c r="J54" s="2"/>
       <c r="K54" s="1"/>
@@ -11243,7 +11341,7 @@
       </c>
       <c r="X54" s="2"/>
       <c r="Y54" s="1">
-        <v>-766176.6</v>
+        <v>-837991.1</v>
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
@@ -11281,9 +11379,11 @@
         <v>0.1</v>
       </c>
       <c r="G55" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H55" s="2"/>
+        <v>78995.5</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="2"/>
       <c r="K55" s="1"/>
@@ -11313,7 +11413,7 @@
       </c>
       <c r="X55" s="2"/>
       <c r="Y55" s="1">
-        <v>-842795.6</v>
+        <v>-921791.1</v>
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
@@ -11351,9 +11451,11 @@
         <v>0.1</v>
       </c>
       <c r="G56" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H56" s="2"/>
+        <v>86895.5</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="2"/>
       <c r="K56" s="1"/>
@@ -11383,7 +11485,7 @@
       </c>
       <c r="X56" s="2"/>
       <c r="Y56" s="1">
-        <v>-927074.7</v>
+        <v>-1013970.2</v>
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
@@ -11421,9 +11523,11 @@
         <v>0.1</v>
       </c>
       <c r="G57" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H57" s="14"/>
+        <v>95585.0</v>
+      </c>
+      <c r="H57" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I57" s="13"/>
       <c r="J57" s="14"/>
       <c r="K57" s="13"/>
@@ -11453,7 +11557,7 @@
       </c>
       <c r="X57" s="14"/>
       <c r="Y57" s="13">
-        <v>-1019782.6</v>
+        <v>-1115367.6</v>
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
@@ -11492,9 +11596,11 @@
         <v>0.1</v>
       </c>
       <c r="G58" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H58" s="2"/>
+        <v>105143.5</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="2"/>
       <c r="K58" s="1"/>
@@ -11524,7 +11630,7 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="1">
-        <v>-1121761.3</v>
+        <v>-1226904.8</v>
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
@@ -11562,9 +11668,11 @@
         <v>0.1</v>
       </c>
       <c r="G59" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H59" s="2"/>
+        <v>115657.5</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="2"/>
       <c r="K59" s="1"/>
@@ -11594,7 +11702,7 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="1">
-        <v>-1233937.8</v>
+        <v>-1349595.3</v>
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
@@ -11632,9 +11740,11 @@
         <v>0.1</v>
       </c>
       <c r="G60" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H60" s="2"/>
+        <v>127223.5</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="2"/>
       <c r="K60" s="1"/>
@@ -11664,7 +11774,7 @@
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="1">
-        <v>-1357331.3</v>
+        <v>-1484554.8</v>
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="1">
@@ -11702,9 +11812,11 @@
         <v>0.1</v>
       </c>
       <c r="G61" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H61" s="2"/>
+        <v>139945.5</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="2"/>
       <c r="K61" s="1"/>
@@ -11734,7 +11846,7 @@
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="1">
-        <v>-1493064.8</v>
+        <v>-1633010.3</v>
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="1">
@@ -11772,9 +11884,11 @@
         <v>0.1</v>
       </c>
       <c r="G62" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H62" s="2"/>
+        <v>153940.0</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="2"/>
       <c r="K62" s="1"/>
@@ -11804,7 +11918,7 @@
       </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="1">
-        <v>-1642371.6</v>
+        <v>-1796311.6</v>
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="1">
@@ -11842,9 +11956,11 @@
         <v>0.1</v>
       </c>
       <c r="G63" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H63" s="2"/>
+        <v>169334.0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="2"/>
       <c r="K63" s="1"/>
@@ -11874,7 +11990,7 @@
       </c>
       <c r="X63" s="2"/>
       <c r="Y63" s="1">
-        <v>-1806609.2</v>
+        <v>-1975943.2</v>
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="1">
@@ -11912,9 +12028,11 @@
         <v>0.1</v>
       </c>
       <c r="G64" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H64" s="2"/>
+        <v>186267.5</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="2"/>
       <c r="K64" s="1"/>
@@ -11944,7 +12062,7 @@
       </c>
       <c r="X64" s="2"/>
       <c r="Y64" s="1">
-        <v>-1987269.7</v>
+        <v>-2173537.2</v>
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="1">
@@ -11982,9 +12100,11 @@
         <v>0.1</v>
       </c>
       <c r="G65" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H65" s="2"/>
+        <v>204894.5</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="2"/>
       <c r="K65" s="1"/>
@@ -12014,7 +12134,7 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" s="1">
-        <v>-2185996.5</v>
+        <v>-2390891.0</v>
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="1">
@@ -12052,9 +12172,11 @@
         <v>0.1</v>
       </c>
       <c r="G66" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H66" s="2"/>
+        <v>225384.0</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="2"/>
       <c r="K66" s="1"/>
@@ -12084,7 +12206,7 @@
       </c>
       <c r="X66" s="2"/>
       <c r="Y66" s="1">
-        <v>-2404596.6</v>
+        <v>-2629980.6</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="1">
@@ -12122,9 +12244,11 @@
         <v>0.1</v>
       </c>
       <c r="G67" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H67" s="2"/>
+        <v>247922.0</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I67" s="1"/>
       <c r="J67" s="2"/>
       <c r="K67" s="1"/>
@@ -12154,7 +12278,7 @@
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" s="1">
-        <v>-2645057.5</v>
+        <v>-2892979.5</v>
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="1">
@@ -12192,9 +12316,11 @@
         <v>0.1</v>
       </c>
       <c r="G68" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="2"/>
+        <v>42382.5</v>
+      </c>
+      <c r="H68" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I68" s="1"/>
       <c r="J68" s="2"/>
       <c r="K68" s="1"/>
@@ -12224,7 +12350,7 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="1">
-        <v>-3370227.2</v>
+        <v>-3412609.7</v>
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="1">
@@ -12262,9 +12388,11 @@
         <v>0.1</v>
       </c>
       <c r="G69" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H69" s="2"/>
+        <v>46621.0</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I69" s="1"/>
       <c r="J69" s="2"/>
       <c r="K69" s="1"/>
@@ -12294,7 +12422,7 @@
       </c>
       <c r="X69" s="2"/>
       <c r="Y69" s="1">
-        <v>-3707249.2</v>
+        <v>-3753870.2</v>
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="1">
@@ -12332,9 +12460,11 @@
         <v>0.1</v>
       </c>
       <c r="G70" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H70" s="2"/>
+        <v>51283.0</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="2"/>
       <c r="K70" s="1"/>
@@ -12364,7 +12494,7 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" s="1">
-        <v>-4077974.1</v>
+        <v>-4129257.1</v>
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="1">
@@ -12402,9 +12532,11 @@
         <v>0.1</v>
       </c>
       <c r="G71" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H71" s="2"/>
+        <v>56411.0</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I71" s="1"/>
       <c r="J71" s="2"/>
       <c r="K71" s="1"/>
@@ -12434,7 +12566,7 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" s="1">
-        <v>-4485772.0</v>
+        <v>-4542183.0</v>
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="1">
@@ -12472,9 +12604,11 @@
         <v>0.1</v>
       </c>
       <c r="G72" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H72" s="16"/>
+        <v>62051.5</v>
+      </c>
+      <c r="H72" s="16">
+        <v>0.5</v>
+      </c>
       <c r="I72" s="5"/>
       <c r="J72" s="16"/>
       <c r="K72" s="5"/>
@@ -12504,7 +12638,7 @@
       </c>
       <c r="X72" s="16"/>
       <c r="Y72" s="5">
-        <v>-4934350.4</v>
+        <v>-4996401.9</v>
       </c>
       <c r="Z72" s="16"/>
       <c r="AA72" s="5">
@@ -17949,7 +18083,7 @@
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="15.282" bestFit="true" customWidth="true" style="0"/>
@@ -18154,7 +18288,9 @@
       <c r="G6" s="1">
         <v>0.0</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
@@ -18222,7 +18358,9 @@
       <c r="G7" s="1">
         <v>0.0</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
@@ -18290,7 +18428,9 @@
       <c r="G8" s="1">
         <v>0.0</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
@@ -18358,7 +18498,9 @@
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
@@ -18426,7 +18568,9 @@
       <c r="G10" s="1">
         <v>0.0</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
@@ -18494,7 +18638,9 @@
       <c r="G11" s="1">
         <v>0.0</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
@@ -18562,7 +18708,9 @@
       <c r="G12" s="1">
         <v>0.0</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
@@ -18630,7 +18778,9 @@
       <c r="G13" s="1">
         <v>0.0</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
@@ -18698,7 +18848,9 @@
       <c r="G14" s="1">
         <v>0.0</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
@@ -18766,7 +18918,9 @@
       <c r="G15" s="1">
         <v>0.0</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
@@ -18834,7 +18988,9 @@
       <c r="G16" s="1">
         <v>0.0</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
@@ -18902,7 +19058,9 @@
       <c r="G17" s="1">
         <v>0.0</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
@@ -18970,7 +19128,9 @@
       <c r="G18" s="1">
         <v>0.0</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
@@ -19038,7 +19198,9 @@
       <c r="G19" s="1">
         <v>0.0</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
@@ -19106,7 +19268,9 @@
       <c r="G20" s="1">
         <v>0.0</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
@@ -19174,7 +19338,9 @@
       <c r="G21" s="1">
         <v>0.0</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
@@ -19242,7 +19408,9 @@
       <c r="G22" s="1">
         <v>0.0</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
@@ -19310,7 +19478,9 @@
       <c r="G23" s="1">
         <v>0.0</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1"/>
@@ -19378,7 +19548,9 @@
       <c r="G24" s="1">
         <v>0.0</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
@@ -19446,7 +19618,9 @@
       <c r="G25" s="1">
         <v>0.0</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="2"/>
       <c r="K25" s="1"/>
@@ -19514,7 +19688,9 @@
       <c r="G26" s="1">
         <v>0.0</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="2"/>
       <c r="K26" s="1"/>
@@ -19582,7 +19758,9 @@
       <c r="G27" s="1">
         <v>0.0</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
@@ -19650,7 +19828,9 @@
       <c r="G28" s="1">
         <v>0.0</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
       <c r="K28" s="1"/>
@@ -19718,7 +19898,9 @@
       <c r="G29" s="1">
         <v>0.0</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1"/>
@@ -19786,7 +19968,9 @@
       <c r="G30" s="1">
         <v>0.0</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
       <c r="K30" s="1"/>
@@ -19854,7 +20038,9 @@
       <c r="G31" s="1">
         <v>0.0</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1"/>
@@ -19922,7 +20108,9 @@
       <c r="G32" s="1">
         <v>0.0</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="2"/>
       <c r="K32" s="1"/>
@@ -19990,7 +20178,9 @@
       <c r="G33" s="1">
         <v>0.0</v>
       </c>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1"/>
@@ -20058,7 +20248,9 @@
       <c r="G34" s="1">
         <v>0.0</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="2"/>
       <c r="K34" s="1"/>
@@ -20126,7 +20318,9 @@
       <c r="G35" s="1">
         <v>0.0</v>
       </c>
-      <c r="H35" s="2"/>
+      <c r="H35" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1"/>
@@ -20194,7 +20388,9 @@
       <c r="G36" s="1">
         <v>0.0</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="2"/>
       <c r="K36" s="1"/>
@@ -20262,7 +20458,9 @@
       <c r="G37" s="1">
         <v>0.0</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1"/>
@@ -20330,7 +20528,9 @@
       <c r="G38" s="1">
         <v>0.0</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="2"/>
       <c r="K38" s="1"/>
@@ -20398,7 +20598,9 @@
       <c r="G39" s="8">
         <v>0.0</v>
       </c>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9">
+        <v>0.5</v>
+      </c>
       <c r="I39" s="8"/>
       <c r="J39" s="9"/>
       <c r="K39" s="8"/>
@@ -20467,7 +20669,9 @@
       <c r="G40" s="11">
         <v>0.0</v>
       </c>
-      <c r="H40" s="12"/>
+      <c r="H40" s="12">
+        <v>0.5</v>
+      </c>
       <c r="I40" s="11"/>
       <c r="J40" s="12"/>
       <c r="K40" s="11"/>
@@ -20536,7 +20740,9 @@
       <c r="G41" s="1">
         <v>0.0</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="2"/>
       <c r="K41" s="1"/>
@@ -20604,7 +20810,9 @@
       <c r="G42" s="1">
         <v>0.0</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="2"/>
       <c r="K42" s="1"/>
@@ -20672,7 +20880,9 @@
       <c r="G43" s="1">
         <v>0.0</v>
       </c>
-      <c r="H43" s="2"/>
+      <c r="H43" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="2"/>
       <c r="K43" s="1"/>
@@ -20740,7 +20950,9 @@
       <c r="G44" s="1">
         <v>0.0</v>
       </c>
-      <c r="H44" s="2"/>
+      <c r="H44" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="2"/>
       <c r="K44" s="1"/>
@@ -20808,7 +21020,9 @@
       <c r="G45" s="1">
         <v>0.0</v>
       </c>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="2"/>
       <c r="K45" s="1"/>
@@ -20876,7 +21090,9 @@
       <c r="G46" s="1">
         <v>0.0</v>
       </c>
-      <c r="H46" s="2"/>
+      <c r="H46" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="2"/>
       <c r="K46" s="1"/>
@@ -20944,7 +21160,9 @@
       <c r="G47" s="1">
         <v>0.0</v>
       </c>
-      <c r="H47" s="2"/>
+      <c r="H47" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="2"/>
       <c r="K47" s="1"/>
@@ -21012,7 +21230,9 @@
       <c r="G48" s="1">
         <v>0.0</v>
       </c>
-      <c r="H48" s="2"/>
+      <c r="H48" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="2"/>
       <c r="K48" s="1"/>
@@ -21080,7 +21300,9 @@
       <c r="G49" s="1">
         <v>0.0</v>
       </c>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="2"/>
       <c r="K49" s="1"/>
@@ -21148,7 +21370,9 @@
       <c r="G50" s="1">
         <v>0.0</v>
       </c>
-      <c r="H50" s="2"/>
+      <c r="H50" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="2"/>
       <c r="K50" s="1"/>
@@ -21216,7 +21440,9 @@
       <c r="G51" s="1">
         <v>0.0</v>
       </c>
-      <c r="H51" s="2"/>
+      <c r="H51" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I51" s="1"/>
       <c r="J51" s="2"/>
       <c r="K51" s="1"/>
@@ -21284,7 +21510,9 @@
       <c r="G52" s="1">
         <v>0.0</v>
       </c>
-      <c r="H52" s="2"/>
+      <c r="H52" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52" s="1"/>
@@ -21352,7 +21580,9 @@
       <c r="G53" s="13">
         <v>0.0</v>
       </c>
-      <c r="H53" s="14"/>
+      <c r="H53" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I53" s="13"/>
       <c r="J53" s="14"/>
       <c r="K53" s="13"/>
@@ -21421,7 +21651,9 @@
       <c r="G54" s="1">
         <v>0.0</v>
       </c>
-      <c r="H54" s="2"/>
+      <c r="H54" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I54" s="1"/>
       <c r="J54" s="2"/>
       <c r="K54" s="1"/>
@@ -21489,7 +21721,9 @@
       <c r="G55" s="1">
         <v>0.0</v>
       </c>
-      <c r="H55" s="2"/>
+      <c r="H55" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="2"/>
       <c r="K55" s="1"/>
@@ -21557,7 +21791,9 @@
       <c r="G56" s="1">
         <v>0.0</v>
       </c>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="2"/>
       <c r="K56" s="1"/>
@@ -21625,9 +21861,11 @@
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H57" s="14"/>
+        <v>99000.0</v>
+      </c>
+      <c r="H57" s="14">
+        <v>0.5</v>
+      </c>
       <c r="I57" s="13"/>
       <c r="J57" s="14"/>
       <c r="K57" s="13"/>
@@ -21657,7 +21895,7 @@
       </c>
       <c r="X57" s="14"/>
       <c r="Y57" s="13">
-        <v>198000.0</v>
+        <v>99000.0</v>
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
@@ -21698,9 +21936,11 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H58" s="2"/>
+        <v>108900.0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="2"/>
       <c r="K58" s="1"/>
@@ -21730,7 +21970,7 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="1">
-        <v>217800.0</v>
+        <v>108900.0</v>
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
@@ -21771,9 +22011,11 @@
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H59" s="2"/>
+        <v>119790.0</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="2"/>
       <c r="K59" s="1"/>
@@ -21803,7 +22045,7 @@
       </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="1">
-        <v>239580.0</v>
+        <v>119790.0</v>
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
@@ -21844,9 +22086,11 @@
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H60" s="2"/>
+        <v>131769.0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="2"/>
       <c r="K60" s="1"/>
@@ -21876,7 +22120,7 @@
       </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="1">
-        <v>263538.0</v>
+        <v>131769.0</v>
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="1">
@@ -21917,9 +22161,11 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H61" s="2"/>
+        <v>144945.9</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="2"/>
       <c r="K61" s="1"/>
@@ -21949,7 +22195,7 @@
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="1">
-        <v>289891.8</v>
+        <v>144945.9</v>
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="1">
@@ -21990,9 +22236,11 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H62" s="2"/>
+        <v>159440.6</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="2"/>
       <c r="K62" s="1"/>
@@ -22022,7 +22270,7 @@
       </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="1">
-        <v>318881.2</v>
+        <v>159440.6</v>
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="1">
@@ -22063,9 +22311,11 @@
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H63" s="2"/>
+        <v>175384.55</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="2"/>
       <c r="K63" s="1"/>
@@ -22095,7 +22345,7 @@
       </c>
       <c r="X63" s="2"/>
       <c r="Y63" s="1">
-        <v>350769.1</v>
+        <v>175384.55</v>
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="1">
@@ -22136,9 +22386,11 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H64" s="2"/>
+        <v>192922.95</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="2"/>
       <c r="K64" s="1"/>
@@ -22168,7 +22420,7 @@
       </c>
       <c r="X64" s="2"/>
       <c r="Y64" s="1">
-        <v>385845.9</v>
+        <v>192922.95</v>
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="1">
@@ -22209,9 +22461,11 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H65" s="2"/>
+        <v>212215.3</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="2"/>
       <c r="K65" s="1"/>
@@ -22241,7 +22495,7 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" s="1">
-        <v>424430.6</v>
+        <v>212215.3</v>
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="1">
@@ -22282,9 +22536,11 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H66" s="2"/>
+        <v>233437.05</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="2"/>
       <c r="K66" s="1"/>
@@ -22314,7 +22570,7 @@
       </c>
       <c r="X66" s="2"/>
       <c r="Y66" s="1">
-        <v>466874.1</v>
+        <v>233437.05</v>
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="1">
@@ -22355,9 +22611,11 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H67" s="2"/>
+        <v>256780.7</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I67" s="1"/>
       <c r="J67" s="2"/>
       <c r="K67" s="1"/>
@@ -22387,7 +22645,7 @@
       </c>
       <c r="X67" s="2"/>
       <c r="Y67" s="1">
-        <v>513561.4</v>
+        <v>256780.7</v>
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="1">
@@ -22428,9 +22686,11 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="2"/>
+        <v>282458.55</v>
+      </c>
+      <c r="H68" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I68" s="1"/>
       <c r="J68" s="2"/>
       <c r="K68" s="1"/>
@@ -22460,7 +22720,7 @@
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="1">
-        <v>564917.1</v>
+        <v>282458.55</v>
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="1">
@@ -22501,9 +22761,11 @@
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H69" s="2"/>
+        <v>310704.35</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I69" s="1"/>
       <c r="J69" s="2"/>
       <c r="K69" s="1"/>
@@ -22533,7 +22795,7 @@
       </c>
       <c r="X69" s="2"/>
       <c r="Y69" s="1">
-        <v>621408.7</v>
+        <v>310704.35</v>
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="1">
@@ -22574,9 +22836,11 @@
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H70" s="2"/>
+        <v>341774.95</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="2"/>
       <c r="K70" s="1"/>
@@ -22606,7 +22870,7 @@
       </c>
       <c r="X70" s="2"/>
       <c r="Y70" s="1">
-        <v>683549.9</v>
+        <v>341774.95</v>
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="1">
@@ -22647,9 +22911,11 @@
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H71" s="2"/>
+        <v>375952.5</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.5</v>
+      </c>
       <c r="I71" s="1"/>
       <c r="J71" s="2"/>
       <c r="K71" s="1"/>
@@ -22679,7 +22945,7 @@
       </c>
       <c r="X71" s="2"/>
       <c r="Y71" s="1">
-        <v>751905.0</v>
+        <v>375952.5</v>
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="1">
@@ -22720,9 +22986,11 @@
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H72" s="16"/>
+        <v>413547.75</v>
+      </c>
+      <c r="H72" s="16">
+        <v>0.5</v>
+      </c>
       <c r="I72" s="5"/>
       <c r="J72" s="16"/>
       <c r="K72" s="5"/>
@@ -22752,7 +23020,7 @@
       </c>
       <c r="X72" s="16"/>
       <c r="Y72" s="5">
-        <v>827095.5</v>
+        <v>413547.75</v>
       </c>
       <c r="Z72" s="16"/>
       <c r="AA72" s="5">

</xml_diff>